<commit_message>
removed short in table of ASDimora
</commit_message>
<xml_diff>
--- a/d/geo--comuni.xlsx
+++ b/d/geo--comuni.xlsx
@@ -22,8 +22,8 @@
     <sheet name="Com_AggrPAFLLavoro" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Comuni!$A$1:$Q$233</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Comuni!$N$1:$AA$234</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Comuni!$A$1:$Q$233</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Comuni!$N$1:$AA$234</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2705" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2688" uniqueCount="662">
   <si>
     <t xml:space="preserve">Chiave</t>
   </si>
@@ -1922,33 +1922,6 @@
   </si>
   <si>
     <t xml:space="preserve">Bezirk Meran</t>
-  </si>
-  <si>
-    <t xml:space="preserve">short</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nn</t>
   </si>
   <si>
     <t xml:space="preserve">Bolzano-città</t>
@@ -2141,7 +2114,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2214,10 +2187,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2234,22 +2203,18 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AD236"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O242" activeCellId="0" sqref="O242"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.71"/>
@@ -2258,7 +2223,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.85"/>
@@ -2272,7 +2237,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="15.57"/>
@@ -2336,7 +2301,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2389,7 +2354,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -2442,7 +2407,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -2495,7 +2460,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -2548,7 +2513,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -2601,7 +2566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -2654,7 +2619,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
@@ -2707,7 +2672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
@@ -2760,7 +2725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
@@ -2813,7 +2778,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -2866,7 +2831,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>48</v>
       </c>
@@ -2919,7 +2884,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -2972,7 +2937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>54</v>
       </c>
@@ -3025,7 +2990,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>57</v>
       </c>
@@ -3078,7 +3043,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>60</v>
       </c>
@@ -3131,7 +3096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>63</v>
       </c>
@@ -3184,7 +3149,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>66</v>
       </c>
@@ -3237,7 +3202,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>69</v>
       </c>
@@ -3290,7 +3255,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>72</v>
       </c>
@@ -3343,7 +3308,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>75</v>
       </c>
@@ -3396,7 +3361,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
         <v>78</v>
       </c>
@@ -3449,7 +3414,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
         <v>81</v>
       </c>
@@ -3502,7 +3467,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
         <v>84</v>
       </c>
@@ -3555,7 +3520,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
         <v>87</v>
       </c>
@@ -3608,7 +3573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
         <v>90</v>
       </c>
@@ -3661,7 +3626,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
         <v>93</v>
       </c>
@@ -3714,7 +3679,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>96</v>
       </c>
@@ -3767,7 +3732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
         <v>99</v>
       </c>
@@ -3820,7 +3785,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>102</v>
       </c>
@@ -3873,7 +3838,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>105</v>
       </c>
@@ -3926,7 +3891,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
         <v>108</v>
       </c>
@@ -3979,7 +3944,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
         <v>111</v>
       </c>
@@ -4032,7 +3997,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>114</v>
       </c>
@@ -4085,7 +4050,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
         <v>117</v>
       </c>
@@ -4138,7 +4103,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
         <v>120</v>
       </c>
@@ -4191,7 +4156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
         <v>123</v>
       </c>
@@ -4244,7 +4209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
         <v>126</v>
       </c>
@@ -4302,7 +4267,7 @@
       <c r="AC38" s="3"/>
       <c r="AD38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
         <v>129</v>
       </c>
@@ -4355,7 +4320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
         <v>132</v>
       </c>
@@ -4408,7 +4373,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
         <v>135</v>
       </c>
@@ -4461,7 +4426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
         <v>138</v>
       </c>
@@ -4514,7 +4479,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
         <v>141</v>
       </c>
@@ -4567,7 +4532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
         <v>144</v>
       </c>
@@ -4620,7 +4585,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
         <v>147</v>
       </c>
@@ -4673,7 +4638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
         <v>150</v>
       </c>
@@ -4726,7 +4691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
         <v>153</v>
       </c>
@@ -4779,7 +4744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
         <v>156</v>
       </c>
@@ -4832,7 +4797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
         <v>159</v>
       </c>
@@ -4885,7 +4850,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
         <v>162</v>
       </c>
@@ -4938,7 +4903,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
         <v>165</v>
       </c>
@@ -4991,7 +4956,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
         <v>168</v>
       </c>
@@ -5044,7 +5009,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
         <v>171</v>
       </c>
@@ -5097,7 +5062,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
         <v>174</v>
       </c>
@@ -5150,7 +5115,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
         <v>177</v>
       </c>
@@ -5203,7 +5168,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
         <v>180</v>
       </c>
@@ -5256,7 +5221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
         <v>183</v>
       </c>
@@ -5309,7 +5274,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
         <v>186</v>
       </c>
@@ -5362,7 +5327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
         <v>189</v>
       </c>
@@ -5415,7 +5380,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
         <v>192</v>
       </c>
@@ -5468,7 +5433,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
         <v>195</v>
       </c>
@@ -5521,7 +5486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
         <v>198</v>
       </c>
@@ -5574,7 +5539,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
         <v>201</v>
       </c>
@@ -5627,7 +5592,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
         <v>204</v>
       </c>
@@ -5680,7 +5645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
         <v>207</v>
       </c>
@@ -5733,7 +5698,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
         <v>210</v>
       </c>
@@ -5786,7 +5751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
         <v>213</v>
       </c>
@@ -5839,7 +5804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
         <v>216</v>
       </c>
@@ -5892,7 +5857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
         <v>219</v>
       </c>
@@ -5945,7 +5910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
         <v>222</v>
       </c>
@@ -5998,7 +5963,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
         <v>225</v>
       </c>
@@ -6051,7 +6016,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
         <v>228</v>
       </c>
@@ -6104,7 +6069,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
         <v>231</v>
       </c>
@@ -6157,7 +6122,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
         <v>234</v>
       </c>
@@ -6210,7 +6175,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
         <v>237</v>
       </c>
@@ -6263,7 +6228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
         <v>240</v>
       </c>
@@ -6316,7 +6281,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
         <v>243</v>
       </c>
@@ -6369,7 +6334,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
         <v>246</v>
       </c>
@@ -6422,7 +6387,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
         <v>249</v>
       </c>
@@ -6475,7 +6440,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
         <v>252</v>
       </c>
@@ -6528,7 +6493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
         <v>255</v>
       </c>
@@ -6581,7 +6546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
         <v>258</v>
       </c>
@@ -6634,7 +6599,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
         <v>261</v>
       </c>
@@ -6687,7 +6652,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
         <v>264</v>
       </c>
@@ -6740,7 +6705,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
         <v>267</v>
       </c>
@@ -6793,7 +6758,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
         <v>270</v>
       </c>
@@ -6846,7 +6811,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
         <v>273</v>
       </c>
@@ -6899,7 +6864,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
         <v>276</v>
       </c>
@@ -6952,7 +6917,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
         <v>279</v>
       </c>
@@ -7005,7 +6970,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
         <v>282</v>
       </c>
@@ -7058,7 +7023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="4" t="s">
         <v>285</v>
       </c>
@@ -7116,7 +7081,7 @@
       <c r="AC91" s="3"/>
       <c r="AD91" s="3"/>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
         <v>288</v>
       </c>
@@ -7169,7 +7134,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
         <v>291</v>
       </c>
@@ -7222,7 +7187,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
         <v>294</v>
       </c>
@@ -7275,7 +7240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
         <v>297</v>
       </c>
@@ -7328,7 +7293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
         <v>300</v>
       </c>
@@ -7381,7 +7346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
         <v>303</v>
       </c>
@@ -7434,7 +7399,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
         <v>306</v>
       </c>
@@ -7487,7 +7452,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
         <v>309</v>
       </c>
@@ -7540,7 +7505,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
         <v>312</v>
       </c>
@@ -7593,7 +7558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
         <v>315</v>
       </c>
@@ -7646,7 +7611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
         <v>318</v>
       </c>
@@ -7699,7 +7664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="s">
         <v>321</v>
       </c>
@@ -7752,7 +7717,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="s">
         <v>324</v>
       </c>
@@ -7805,7 +7770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="s">
         <v>327</v>
       </c>
@@ -7858,7 +7823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="s">
         <v>330</v>
       </c>
@@ -7911,7 +7876,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="s">
         <v>333</v>
       </c>
@@ -8017,7 +7982,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="s">
         <v>339</v>
       </c>
@@ -8070,7 +8035,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="s">
         <v>342</v>
       </c>
@@ -8123,7 +8088,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="s">
         <v>345</v>
       </c>
@@ -8176,7 +8141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="s">
         <v>348</v>
       </c>
@@ -8229,7 +8194,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="s">
         <v>351</v>
       </c>
@@ -8282,7 +8247,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="2" t="s">
         <v>354</v>
       </c>
@@ -8335,7 +8300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="2" t="s">
         <v>357</v>
       </c>
@@ -8388,7 +8353,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="2" t="s">
         <v>360</v>
       </c>
@@ -8441,7 +8406,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="12" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="2" t="s">
         <v>363</v>
       </c>
@@ -8494,7 +8459,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="2" t="s">
         <v>33</v>
       </c>
@@ -8547,7 +8512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="2" t="s">
         <v>339</v>
       </c>
@@ -8600,7 +8565,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="2" t="s">
         <v>17</v>
       </c>
@@ -8653,7 +8618,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="2" t="s">
         <v>132</v>
       </c>
@@ -8706,7 +8671,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="2" t="s">
         <v>24</v>
       </c>
@@ -8759,7 +8724,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="2" t="s">
         <v>21</v>
       </c>
@@ -8812,7 +8777,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="2" t="s">
         <v>198</v>
       </c>
@@ -8865,7 +8830,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="2" t="s">
         <v>36</v>
       </c>
@@ -8918,7 +8883,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="2" t="s">
         <v>39</v>
       </c>
@@ -8971,7 +8936,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="2" t="s">
         <v>51</v>
       </c>
@@ -9024,7 +8989,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="s">
         <v>45</v>
       </c>
@@ -9077,7 +9042,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="s">
         <v>48</v>
       </c>
@@ -9130,7 +9095,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="2" t="s">
         <v>54</v>
       </c>
@@ -9183,7 +9148,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="2" t="s">
         <v>216</v>
       </c>
@@ -9236,7 +9201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="2" t="s">
         <v>93</v>
       </c>
@@ -9289,7 +9254,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="2" t="s">
         <v>195</v>
       </c>
@@ -9342,7 +9307,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="2" t="s">
         <v>159</v>
       </c>
@@ -9395,7 +9360,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="2" t="s">
         <v>27</v>
       </c>
@@ -9448,7 +9413,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="2" t="s">
         <v>351</v>
       </c>
@@ -9501,7 +9466,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="2" t="s">
         <v>111</v>
       </c>
@@ -9554,7 +9519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="2" t="s">
         <v>63</v>
       </c>
@@ -9607,7 +9572,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="2" t="s">
         <v>117</v>
       </c>
@@ -9660,7 +9625,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="2" t="s">
         <v>120</v>
       </c>
@@ -9713,7 +9678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="2" t="s">
         <v>123</v>
       </c>
@@ -9766,7 +9731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="2" t="s">
         <v>96</v>
       </c>
@@ -9819,7 +9784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="2" t="s">
         <v>342</v>
       </c>
@@ -9872,7 +9837,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="2" t="s">
         <v>30</v>
       </c>
@@ -9925,7 +9890,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="2" t="s">
         <v>249</v>
       </c>
@@ -9978,7 +9943,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="2" t="s">
         <v>252</v>
       </c>
@@ -10031,7 +9996,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="2" t="s">
         <v>60</v>
       </c>
@@ -10084,7 +10049,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="2" t="s">
         <v>84</v>
       </c>
@@ -10137,7 +10102,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="2" t="s">
         <v>69</v>
       </c>
@@ -10190,7 +10155,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="2" t="s">
         <v>72</v>
       </c>
@@ -10243,7 +10208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="2" t="s">
         <v>78</v>
       </c>
@@ -10296,7 +10261,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="2" t="s">
         <v>81</v>
       </c>
@@ -10349,7 +10314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="2" t="s">
         <v>57</v>
       </c>
@@ -10402,7 +10367,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="2" t="s">
         <v>87</v>
       </c>
@@ -10455,7 +10420,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="2" t="s">
         <v>90</v>
       </c>
@@ -10508,7 +10473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="2" t="s">
         <v>144</v>
       </c>
@@ -10561,7 +10526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="2" t="s">
         <v>135</v>
       </c>
@@ -10614,7 +10579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="2" t="s">
         <v>141</v>
       </c>
@@ -10667,7 +10632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="2" t="s">
         <v>129</v>
       </c>
@@ -10720,7 +10685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="2" t="s">
         <v>147</v>
       </c>
@@ -10773,7 +10738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="2" t="s">
         <v>138</v>
       </c>
@@ -10826,7 +10791,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="2" t="s">
         <v>150</v>
       </c>
@@ -10879,7 +10844,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="2" t="s">
         <v>156</v>
       </c>
@@ -10932,7 +10897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="2" t="s">
         <v>153</v>
       </c>
@@ -10985,7 +10950,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="2" t="s">
         <v>162</v>
       </c>
@@ -11038,7 +11003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="2" t="s">
         <v>165</v>
       </c>
@@ -11091,7 +11056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="2" t="s">
         <v>171</v>
       </c>
@@ -11144,7 +11109,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="2" t="s">
         <v>168</v>
       </c>
@@ -11197,7 +11162,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="2" t="s">
         <v>177</v>
       </c>
@@ -11250,7 +11215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="2" t="s">
         <v>180</v>
       </c>
@@ -11303,7 +11268,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="2" t="s">
         <v>240</v>
       </c>
@@ -11356,7 +11321,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="2" t="s">
         <v>279</v>
       </c>
@@ -11409,7 +11374,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="2" t="s">
         <v>183</v>
       </c>
@@ -11462,7 +11427,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="2" t="s">
         <v>186</v>
       </c>
@@ -11515,7 +11480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="2" t="s">
         <v>189</v>
       </c>
@@ -11568,7 +11533,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="2" t="s">
         <v>102</v>
       </c>
@@ -11621,7 +11586,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="2" t="s">
         <v>357</v>
       </c>
@@ -11674,7 +11639,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="2" t="s">
         <v>333</v>
       </c>
@@ -11727,7 +11692,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="2" t="s">
         <v>204</v>
       </c>
@@ -11780,7 +11745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="2" t="s">
         <v>207</v>
       </c>
@@ -11833,7 +11798,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="2" t="s">
         <v>105</v>
       </c>
@@ -11886,7 +11851,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="2" t="s">
         <v>330</v>
       </c>
@@ -11992,7 +11957,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="2" t="s">
         <v>210</v>
       </c>
@@ -12045,7 +12010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="2" t="s">
         <v>219</v>
       </c>
@@ -12098,7 +12063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="2" t="s">
         <v>42</v>
       </c>
@@ -12151,7 +12116,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="2" t="s">
         <v>222</v>
       </c>
@@ -12204,7 +12169,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="2" t="s">
         <v>225</v>
       </c>
@@ -12257,7 +12222,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="2" t="s">
         <v>231</v>
       </c>
@@ -12310,7 +12275,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="2" t="s">
         <v>228</v>
       </c>
@@ -12363,7 +12328,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="2" t="s">
         <v>237</v>
       </c>
@@ -12416,7 +12381,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="2" t="s">
         <v>234</v>
       </c>
@@ -12469,7 +12434,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="2" t="s">
         <v>243</v>
       </c>
@@ -12522,7 +12487,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="2" t="s">
         <v>246</v>
       </c>
@@ -12575,7 +12540,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="2" t="s">
         <v>66</v>
       </c>
@@ -12628,7 +12593,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="2" t="s">
         <v>273</v>
       </c>
@@ -12681,7 +12646,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="2" t="s">
         <v>276</v>
       </c>
@@ -12734,7 +12699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="2" t="s">
         <v>294</v>
       </c>
@@ -12787,7 +12752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="2" t="s">
         <v>297</v>
       </c>
@@ -12840,7 +12805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="2" t="s">
         <v>288</v>
       </c>
@@ -12893,7 +12858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="2" t="s">
         <v>291</v>
       </c>
@@ -12946,7 +12911,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="2" t="s">
         <v>270</v>
       </c>
@@ -12999,7 +12964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="2" t="s">
         <v>255</v>
       </c>
@@ -13052,7 +13017,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="2" t="s">
         <v>258</v>
       </c>
@@ -13105,7 +13070,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="2" t="s">
         <v>264</v>
       </c>
@@ -13158,7 +13123,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="2" t="s">
         <v>261</v>
       </c>
@@ -13211,7 +13176,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="2" t="s">
         <v>267</v>
       </c>
@@ -13264,7 +13229,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="2" t="s">
         <v>201</v>
       </c>
@@ -13317,7 +13282,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="2" t="s">
         <v>363</v>
       </c>
@@ -13370,7 +13335,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="2" t="s">
         <v>300</v>
       </c>
@@ -13423,7 +13388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="2" t="s">
         <v>324</v>
       </c>
@@ -13476,7 +13441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="2" t="s">
         <v>303</v>
       </c>
@@ -13529,7 +13494,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="2" t="s">
         <v>306</v>
       </c>
@@ -13582,7 +13547,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="2" t="s">
         <v>315</v>
       </c>
@@ -13635,7 +13600,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="2" t="s">
         <v>318</v>
       </c>
@@ -13688,7 +13653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="216" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="2" t="s">
         <v>312</v>
       </c>
@@ -13741,7 +13706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="2" t="s">
         <v>99</v>
       </c>
@@ -13794,7 +13759,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="2" t="s">
         <v>309</v>
       </c>
@@ -13847,7 +13812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="2" t="s">
         <v>321</v>
       </c>
@@ -13900,7 +13865,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="2" t="s">
         <v>75</v>
       </c>
@@ -13953,7 +13918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="2" t="s">
         <v>327</v>
       </c>
@@ -14006,7 +13971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="2" t="s">
         <v>285</v>
       </c>
@@ -14059,7 +14024,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="2" t="s">
         <v>348</v>
       </c>
@@ -14112,7 +14077,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="224" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="2" t="s">
         <v>360</v>
       </c>
@@ -14165,7 +14130,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="2" t="s">
         <v>114</v>
       </c>
@@ -14218,7 +14183,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="226" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="2" t="s">
         <v>345</v>
       </c>
@@ -14271,7 +14236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="2" t="s">
         <v>108</v>
       </c>
@@ -14324,7 +14289,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="228" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="2" t="s">
         <v>354</v>
       </c>
@@ -14377,7 +14342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="229" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="2" t="s">
         <v>213</v>
       </c>
@@ -14430,7 +14395,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="230" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="2" t="s">
         <v>174</v>
       </c>
@@ -14483,7 +14448,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="231" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="2" t="s">
         <v>192</v>
       </c>
@@ -14536,7 +14501,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="2" t="s">
         <v>126</v>
       </c>
@@ -14589,7 +14554,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="2" t="s">
         <v>282</v>
       </c>
@@ -14733,14 +14698,6 @@
       <c r="AD236" s="15"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q233">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="107 Pfitsch"/>
-        <filter val="107 Val di Vizze"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -14748,7 +14705,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14763,7 +14719,7 @@
       <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.71"/>
@@ -14922,7 +14878,7 @@
       <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.71"/>
@@ -14948,7 +14904,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>668</v>
+        <v>659</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15025,7 +14981,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>669</v>
+        <v>660</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15201,7 +15157,7 @@
         <v>366</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>670</v>
+        <v>661</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15314,7 +15270,7 @@
       <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.57"/>
@@ -15340,7 +15296,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>668</v>
+        <v>659</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15417,7 +15373,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>669</v>
+        <v>660</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15593,7 +15549,7 @@
         <v>366</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>670</v>
+        <v>661</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15709,14 +15665,14 @@
       <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16161,7 +16117,7 @@
       <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.42"/>
@@ -16429,12 +16385,12 @@
       <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16747,20 +16703,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
         <v>12</v>
       </c>
@@ -16770,11 +16727,8 @@
       <c r="C1" s="5" t="s">
         <v>591</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="n">
         <v>1</v>
       </c>
@@ -16784,11 +16738,8 @@
       <c r="C2" s="0" t="s">
         <v>623</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="n">
         <v>2</v>
       </c>
@@ -16798,11 +16749,8 @@
       <c r="C3" s="0" t="s">
         <v>625</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="n">
         <v>3</v>
       </c>
@@ -16812,11 +16760,8 @@
       <c r="C4" s="0" t="s">
         <v>599</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="n">
         <v>4</v>
       </c>
@@ -16826,11 +16771,8 @@
       <c r="C5" s="0" t="s">
         <v>601</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="n">
         <v>5</v>
       </c>
@@ -16840,11 +16782,8 @@
       <c r="C6" s="0" t="s">
         <v>603</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="n">
         <v>6</v>
       </c>
@@ -16854,11 +16793,8 @@
       <c r="C7" s="0" t="s">
         <v>605</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="n">
         <v>7</v>
       </c>
@@ -16868,11 +16804,8 @@
       <c r="C8" s="0" t="s">
         <v>607</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
         <v>609</v>
       </c>
@@ -16882,11 +16815,8 @@
       <c r="C9" s="0" t="s">
         <v>611</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="n">
         <v>1</v>
       </c>
@@ -16896,11 +16826,8 @@
       <c r="C10" s="0" t="s">
         <v>627</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="n">
         <v>2</v>
       </c>
@@ -16910,11 +16837,8 @@
       <c r="C11" s="0" t="s">
         <v>628</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="n">
         <v>3</v>
       </c>
@@ -16924,11 +16848,8 @@
       <c r="C12" s="0" t="s">
         <v>616</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="n">
         <v>4</v>
       </c>
@@ -16938,11 +16859,8 @@
       <c r="C13" s="0" t="s">
         <v>617</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="n">
         <v>5</v>
       </c>
@@ -16952,11 +16870,8 @@
       <c r="C14" s="0" t="s">
         <v>618</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="n">
         <v>6</v>
       </c>
@@ -16966,11 +16881,8 @@
       <c r="C15" s="0" t="s">
         <v>619</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="n">
         <v>7</v>
       </c>
@@ -16980,11 +16892,8 @@
       <c r="C16" s="0" t="s">
         <v>620</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
         <v>609</v>
       </c>
@@ -16993,9 +16902,6 @@
       </c>
       <c r="C17" s="0" t="s">
         <v>622</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>637</v>
       </c>
     </row>
   </sheetData>
@@ -17020,7 +16926,7 @@
       <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.71"/>
@@ -17029,7 +16935,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="6" t="s">
@@ -17053,7 +16959,7 @@
         <v>595</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>638</v>
+        <v>629</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17064,10 +16970,10 @@
         <v>18</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>639</v>
+        <v>630</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>640</v>
+        <v>631</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17081,7 +16987,7 @@
         <v>597</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>641</v>
+        <v>632</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17092,10 +16998,10 @@
         <v>18</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>642</v>
+        <v>633</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>643</v>
+        <v>634</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17120,10 +17026,10 @@
         <v>18</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>644</v>
+        <v>635</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>645</v>
+        <v>636</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17151,7 +17057,7 @@
         <v>612</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>646</v>
+        <v>637</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17162,10 +17068,10 @@
         <v>366</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>647</v>
+        <v>638</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>648</v>
+        <v>639</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17179,7 +17085,7 @@
         <v>614</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>649</v>
+        <v>640</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17190,10 +17096,10 @@
         <v>366</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17218,10 +17124,10 @@
         <v>366</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>652</v>
+        <v>643</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>653</v>
+        <v>644</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17263,7 +17169,7 @@
       <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.86"/>
@@ -17288,7 +17194,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>654</v>
+        <v>645</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17299,7 +17205,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17310,7 +17216,7 @@
         <v>18</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>656</v>
+        <v>647</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17332,7 +17238,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>657</v>
+        <v>648</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17343,7 +17249,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>658</v>
+        <v>649</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17354,7 +17260,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>659</v>
+        <v>650</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17365,7 +17271,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>660</v>
+        <v>651</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17387,7 +17293,7 @@
         <v>366</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>661</v>
+        <v>652</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17398,7 +17304,7 @@
         <v>366</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>662</v>
+        <v>653</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17409,7 +17315,7 @@
         <v>366</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>663</v>
+        <v>654</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17431,7 +17337,7 @@
         <v>366</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>664</v>
+        <v>655</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17442,7 +17348,7 @@
         <v>366</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>665</v>
+        <v>656</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17453,7 +17359,7 @@
         <v>366</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>666</v>
+        <v>657</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17464,7 +17370,7 @@
         <v>366</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>667</v>
+        <v>658</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17500,7 +17406,7 @@
       <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
@@ -17521,7 +17427,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>654</v>
+        <v>645</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17532,7 +17438,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17543,7 +17449,7 @@
         <v>18</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>656</v>
+        <v>647</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17565,7 +17471,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>657</v>
+        <v>648</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17576,7 +17482,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>658</v>
+        <v>649</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17587,7 +17493,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>659</v>
+        <v>650</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17598,7 +17504,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>660</v>
+        <v>651</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17620,7 +17526,7 @@
         <v>366</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>661</v>
+        <v>652</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17631,7 +17537,7 @@
         <v>366</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>662</v>
+        <v>653</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17642,7 +17548,7 @@
         <v>366</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>663</v>
+        <v>654</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17664,7 +17570,7 @@
         <v>366</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>664</v>
+        <v>655</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17675,7 +17581,7 @@
         <v>366</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>665</v>
+        <v>656</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17686,7 +17592,7 @@
         <v>366</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>666</v>
+        <v>657</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17697,7 +17603,7 @@
         <v>366</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>667</v>
+        <v>658</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17733,7 +17639,7 @@
       <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">

</xml_diff>

<commit_message>
# tab label in formato long
</commit_message>
<xml_diff>
--- a/d/geo--comuni.xlsx
+++ b/d/geo--comuni.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\AMB\ARBDATEN\OnlineGrafiken\motioncharts\d\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\PROGETTO\COVID\Covid-2\motioncharts\d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBDF124-72B8-4902-9665-866E9A7C0076}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568856D0-FB21-4F25-93B1-F5794EBB0813}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="682" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="682" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comuni" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,11 @@
     <sheet name="Com_AggrASLLavoro" sheetId="10" r:id="rId10"/>
     <sheet name="Com_AggrPAFDimora" sheetId="11" r:id="rId11"/>
     <sheet name="Com_AggrPAFLLavoro" sheetId="12" r:id="rId12"/>
+    <sheet name="Label" sheetId="13" r:id="rId13"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Comuni!$A$1:$R$233</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="0">Comuni!$O$1:$AB$233</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Comuni!$A$1:$R$233</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3358" uniqueCount="843">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3385" uniqueCount="857">
   <si>
     <t>Chiave</t>
   </si>
@@ -2569,13 +2570,55 @@
   </si>
   <si>
     <t>#8B0000</t>
+  </si>
+  <si>
+    <t>Valore</t>
+  </si>
+  <si>
+    <t>ydesc</t>
+  </si>
+  <si>
+    <t>xdesc</t>
+  </si>
+  <si>
+    <t>main.title</t>
+  </si>
+  <si>
+    <t>main.title2</t>
+  </si>
+  <si>
+    <t>Neue_Positive</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Neue Tägliche Fallzahlen</t>
+  </si>
+  <si>
+    <t>Gesamte Tägliche Fallzahlen</t>
+  </si>
+  <si>
+    <t>Nuovi contagi giornalieri</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Totale contagi giornalieri</t>
+  </si>
+  <si>
+    <t>Nuovi positivi</t>
+  </si>
+  <si>
+    <t>Label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2591,6 +2634,11 @@
       <sz val="8"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2625,7 +2673,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2641,9 +2689,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2659,7 +2708,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2957,11 +3006,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G187" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N118" sqref="N118:N233"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -16771,7 +16820,7 @@
       <selection activeCell="D2" sqref="D2:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -16949,7 +16998,7 @@
       <selection activeCell="D2" sqref="D2:D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -17426,7 +17475,7 @@
       <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
@@ -17895,6 +17944,145 @@
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95382AF-4388-452A-9731-96532A40BD57}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>844</v>
+      </c>
+      <c r="B2" t="s">
+        <v>366</v>
+      </c>
+      <c r="C2" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>845</v>
+      </c>
+      <c r="B3" t="s">
+        <v>366</v>
+      </c>
+      <c r="C3" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>846</v>
+      </c>
+      <c r="B4" t="s">
+        <v>366</v>
+      </c>
+      <c r="C4" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>847</v>
+      </c>
+      <c r="B5" t="s">
+        <v>366</v>
+      </c>
+      <c r="C5" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>844</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>845</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>846</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>847</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="11"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="11"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -17906,7 +18094,7 @@
       <selection activeCell="G12" sqref="G12:G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -18407,7 +18595,7 @@
       <selection activeCell="E10" sqref="E10:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -18712,7 +18900,7 @@
       <selection activeCell="E2" sqref="E2:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -19085,7 +19273,7 @@
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
@@ -19339,7 +19527,7 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -19613,7 +19801,7 @@
       <selection activeCell="D2" sqref="D2:D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="30.85546875" customWidth="1"/>
@@ -19893,7 +20081,7 @@
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="22.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="22.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
@@ -20169,7 +20357,7 @@
       <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>

</xml_diff>

<commit_message>
## aggiunta lingua Spagnolo, Francese
</commit_message>
<xml_diff>
--- a/d/geo--comuni.xlsx
+++ b/d/geo--comuni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\PROGETTO\COVID\Covid-2\motioncharts\d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568856D0-FB21-4F25-93B1-F5794EBB0813}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE37516-5713-43F6-B519-1BB1D271078D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="682" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3385" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3421" uniqueCount="871">
   <si>
     <t>Chiave</t>
   </si>
@@ -2612,6 +2612,48 @@
   </si>
   <si>
     <t>Label</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>New Positives</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>New Covid-19 cases per day</t>
+  </si>
+  <si>
+    <t>Total Covid-19 cases per day</t>
+  </si>
+  <si>
+    <t>Français</t>
+  </si>
+  <si>
+    <t>Total des cas de Covid-19 par jour</t>
+  </si>
+  <si>
+    <t>Noveaux cas de Covid-19 par jour</t>
+  </si>
+  <si>
+    <t>Noveaux cas positifs par jour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Español </t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nuevos Casos Positivos Covid -19 </t>
+  </si>
+  <si>
+    <t>Nuevos casos diarios de Covid-19</t>
+  </si>
+  <si>
+    <t>Total de casos diarios de Covid-19</t>
   </si>
 </sst>
 </file>
@@ -17949,17 +17991,17 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95382AF-4388-452A-9731-96532A40BD57}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -18061,23 +18103,137 @@
         <v>854</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>844</v>
+      </c>
+      <c r="B10" t="s">
+        <v>857</v>
+      </c>
+      <c r="C10" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>845</v>
+      </c>
+      <c r="B11" t="s">
+        <v>857</v>
+      </c>
+      <c r="C11" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>846</v>
+      </c>
+      <c r="B12" t="s">
+        <v>857</v>
+      </c>
+      <c r="C12" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>847</v>
+      </c>
+      <c r="B13" t="s">
+        <v>857</v>
+      </c>
+      <c r="C13" t="s">
+        <v>861</v>
+      </c>
+    </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
+      <c r="A14" t="s">
+        <v>844</v>
+      </c>
+      <c r="B14" t="s">
+        <v>862</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
+      <c r="A15" t="s">
+        <v>845</v>
+      </c>
+      <c r="B15" t="s">
+        <v>862</v>
+      </c>
+      <c r="C15" t="s">
+        <v>859</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="11"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="11"/>
+      <c r="A16" t="s">
+        <v>846</v>
+      </c>
+      <c r="B16" t="s">
+        <v>862</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>847</v>
+      </c>
+      <c r="B17" t="s">
+        <v>862</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>844</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>866</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>845</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>866</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>846</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>866</v>
+      </c>
+      <c r="C20" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>847</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>866</v>
+      </c>
+      <c r="C21" t="s">
+        <v>870</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
# modifiche foglio Label
</commit_message>
<xml_diff>
--- a/d/geo--comuni.xlsx
+++ b/d/geo--comuni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\PROGETTO\COVID\Covid-2\motioncharts\d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE37516-5713-43F6-B519-1BB1D271078D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C69002-EC2E-45FC-A2A7-1BF6A78E75EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="682" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3421" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3388" uniqueCount="869">
   <si>
     <t>Chiave</t>
   </si>
@@ -2572,9 +2572,6 @@
     <t>#8B0000</t>
   </si>
   <si>
-    <t>Valore</t>
-  </si>
-  <si>
     <t>ydesc</t>
   </si>
   <si>
@@ -2609,9 +2606,6 @@
   </si>
   <si>
     <t>Nuovi positivi</t>
-  </si>
-  <si>
-    <t>Label</t>
   </si>
   <si>
     <t>English</t>
@@ -17991,248 +17985,119 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95382AF-4388-452A-9731-96532A40BD57}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E1" t="s">
+        <v>860</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>843</v>
+      </c>
+      <c r="B2" t="s">
+        <v>847</v>
+      </c>
+      <c r="C2" t="s">
+        <v>854</v>
+      </c>
+      <c r="D2" t="s">
         <v>856</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="E2" s="11" t="s">
+        <v>863</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>844</v>
       </c>
-      <c r="B2" t="s">
-        <v>366</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>848</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>852</v>
+      </c>
+      <c r="D3" t="s">
+        <v>857</v>
+      </c>
+      <c r="E3" t="s">
+        <v>857</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>845</v>
       </c>
-      <c r="B3" t="s">
-        <v>366</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
+        <v>851</v>
+      </c>
+      <c r="D4" t="s">
+        <v>858</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>862</v>
+      </c>
+      <c r="F4" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>846</v>
       </c>
-      <c r="B4" t="s">
-        <v>366</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B5" t="s">
         <v>850</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>847</v>
-      </c>
-      <c r="B5" t="s">
-        <v>366</v>
-      </c>
       <c r="C5" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>844</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>845</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
         <v>853</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>846</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>847</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>844</v>
-      </c>
-      <c r="B10" t="s">
-        <v>857</v>
-      </c>
-      <c r="C10" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>845</v>
-      </c>
-      <c r="B11" t="s">
-        <v>857</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D5" t="s">
         <v>859</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>846</v>
-      </c>
-      <c r="B12" t="s">
-        <v>857</v>
-      </c>
-      <c r="C12" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>847</v>
-      </c>
-      <c r="B13" t="s">
-        <v>857</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="E5" s="11" t="s">
         <v>861</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>844</v>
-      </c>
-      <c r="B14" t="s">
-        <v>862</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>845</v>
-      </c>
-      <c r="B15" t="s">
-        <v>862</v>
-      </c>
-      <c r="C15" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>846</v>
-      </c>
-      <c r="B16" t="s">
-        <v>862</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>847</v>
-      </c>
-      <c r="B17" t="s">
-        <v>862</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>844</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>866</v>
-      </c>
-      <c r="C18" s="11" t="s">
+      <c r="F5" t="s">
         <v>868</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>845</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>866</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>846</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>866</v>
-      </c>
-      <c r="C20" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>847</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>866</v>
-      </c>
-      <c r="C21" t="s">
-        <v>870</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
# Neues Tab "Wetter_Station"
</commit_message>
<xml_diff>
--- a/d/geo--comuni.xlsx
+++ b/d/geo--comuni.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\PROGETTO\COVID\Covid-2\motioncharts\d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C69002-EC2E-45FC-A2A7-1BF6A78E75EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB851DAA-D0FB-4AE2-A194-6D731EA8B139}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="682" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="682" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comuni" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="Com_AggrPAFDimora" sheetId="11" r:id="rId11"/>
     <sheet name="Com_AggrPAFLLavoro" sheetId="12" r:id="rId12"/>
     <sheet name="Label" sheetId="13" r:id="rId13"/>
+    <sheet name="Wetter_station" sheetId="14" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Comuni!$A$1:$R$233</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3388" uniqueCount="869">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3858" uniqueCount="940">
   <si>
     <t>Chiave</t>
   </si>
@@ -2648,6 +2649,219 @@
   </si>
   <si>
     <t>Total de casos diarios de Covid-19</t>
+  </si>
+  <si>
+    <t>Wetter_station</t>
+  </si>
+  <si>
+    <t>03100MS</t>
+  </si>
+  <si>
+    <t>06400MS</t>
+  </si>
+  <si>
+    <t>08200MS</t>
+  </si>
+  <si>
+    <t>02200MS</t>
+  </si>
+  <si>
+    <t>02500MS</t>
+  </si>
+  <si>
+    <t>37100MS</t>
+  </si>
+  <si>
+    <t>86900MS</t>
+  </si>
+  <si>
+    <t>83200MS</t>
+  </si>
+  <si>
+    <t>41000MS</t>
+  </si>
+  <si>
+    <t>59700MS</t>
+  </si>
+  <si>
+    <t>50500MS</t>
+  </si>
+  <si>
+    <t>88820MS</t>
+  </si>
+  <si>
+    <t>87300MS</t>
+  </si>
+  <si>
+    <t>85700MS</t>
+  </si>
+  <si>
+    <t>09700MS</t>
+  </si>
+  <si>
+    <t>11400MS</t>
+  </si>
+  <si>
+    <t>Hintermartell</t>
+  </si>
+  <si>
+    <t>19300MS</t>
+  </si>
+  <si>
+    <t>15800MS</t>
+  </si>
+  <si>
+    <t>Schnals Vernagt</t>
+  </si>
+  <si>
+    <t>Laas - Eyrs</t>
+  </si>
+  <si>
+    <t>Taufers i.M.</t>
+  </si>
+  <si>
+    <t>Marienberg</t>
+  </si>
+  <si>
+    <t>St. Valentin a.d. Haide</t>
+  </si>
+  <si>
+    <t>23200MS</t>
+  </si>
+  <si>
+    <t>27100MS</t>
+  </si>
+  <si>
+    <t>Sulden</t>
+  </si>
+  <si>
+    <t>25900MS</t>
+  </si>
+  <si>
+    <t>St. Walburg</t>
+  </si>
+  <si>
+    <t>24400MS</t>
+  </si>
+  <si>
+    <t>Ulten Weißbrunn</t>
+  </si>
+  <si>
+    <t>22210MS</t>
+  </si>
+  <si>
+    <t>St. Martin in Passeier</t>
+  </si>
+  <si>
+    <t>89190MS</t>
+  </si>
+  <si>
+    <t>Kaltern Oberplanitzing</t>
+  </si>
+  <si>
+    <t>Bozen(?)</t>
+  </si>
+  <si>
+    <t>Barbian Kollmann</t>
+  </si>
+  <si>
+    <t>74900MS</t>
+  </si>
+  <si>
+    <t>75600MS</t>
+  </si>
+  <si>
+    <t>78305MS</t>
+  </si>
+  <si>
+    <t>85120MS</t>
+  </si>
+  <si>
+    <t>82910MS</t>
+  </si>
+  <si>
+    <t>82200MS</t>
+  </si>
+  <si>
+    <t>Sarnthein</t>
+  </si>
+  <si>
+    <t>Radein</t>
+  </si>
+  <si>
+    <t>Wolkenstein</t>
+  </si>
+  <si>
+    <t>73500MS</t>
+  </si>
+  <si>
+    <t>Brixen Vahrn</t>
+  </si>
+  <si>
+    <t>39100MS</t>
+  </si>
+  <si>
+    <t>Franzensfeste Grasstein</t>
+  </si>
+  <si>
+    <t>37700MS</t>
+  </si>
+  <si>
+    <t>Obervintl</t>
+  </si>
+  <si>
+    <t>65350MS</t>
+  </si>
+  <si>
+    <t>Pfitsch St. Jakob</t>
+  </si>
+  <si>
+    <t>33500MS</t>
+  </si>
+  <si>
+    <t>St. Veit in Prags</t>
+  </si>
+  <si>
+    <t>42700MS</t>
+  </si>
+  <si>
+    <t>Sand i.T. Mühlen</t>
+  </si>
+  <si>
+    <t>56900MS</t>
+  </si>
+  <si>
+    <t>Welsberg</t>
+  </si>
+  <si>
+    <t>43200MS</t>
+  </si>
+  <si>
+    <t>Antholz Obertal</t>
+  </si>
+  <si>
+    <t>47400MS</t>
+  </si>
+  <si>
+    <t>65600MS</t>
+  </si>
+  <si>
+    <t>St. Magdalena in Gsies</t>
+  </si>
+  <si>
+    <t>44500MS</t>
+  </si>
+  <si>
+    <t>56500MS</t>
+  </si>
+  <si>
+    <t>St. Martin in Thurn</t>
+  </si>
+  <si>
+    <t>62600MS</t>
+  </si>
+  <si>
+    <t>Wetter_station_NAME</t>
   </si>
 </sst>
 </file>
@@ -2677,7 +2891,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2696,6 +2910,18 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2709,7 +2935,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2726,6 +2952,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3042,8 +3274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE233"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17987,7 +18219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95382AF-4388-452A-9731-96532A40BD57}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -18102,6 +18334,2024 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBDBBA6-5C55-4D9B-AB4F-2CB9A3B7975E}">
+  <dimension ref="A1:F117"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>873</v>
+      </c>
+      <c r="E2" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>874</v>
+      </c>
+      <c r="E3" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>874</v>
+      </c>
+      <c r="E4" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>872</v>
+      </c>
+      <c r="E5" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>872</v>
+      </c>
+      <c r="E6" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>871</v>
+      </c>
+      <c r="E7" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>870</v>
+      </c>
+      <c r="E8" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>874</v>
+      </c>
+      <c r="E9" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>872</v>
+      </c>
+      <c r="E10" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>885</v>
+      </c>
+      <c r="E11" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>884</v>
+      </c>
+      <c r="E12" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>887</v>
+      </c>
+      <c r="E13" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>887</v>
+      </c>
+      <c r="E14" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>888</v>
+      </c>
+      <c r="E15" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>894</v>
+      </c>
+      <c r="E16" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>894</v>
+      </c>
+      <c r="E17" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>894</v>
+      </c>
+      <c r="E18" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>895</v>
+      </c>
+      <c r="E19" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>894</v>
+      </c>
+      <c r="E20" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>894</v>
+      </c>
+      <c r="E21" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>894</v>
+      </c>
+      <c r="E22" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>894</v>
+      </c>
+      <c r="E23" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>887</v>
+      </c>
+      <c r="E24" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>895</v>
+      </c>
+      <c r="E25" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>894</v>
+      </c>
+      <c r="E26" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>894</v>
+      </c>
+      <c r="E27" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>894</v>
+      </c>
+      <c r="E28" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>895</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>895</v>
+      </c>
+      <c r="E30" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>897</v>
+      </c>
+      <c r="E31" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>897</v>
+      </c>
+      <c r="E32" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>897</v>
+      </c>
+      <c r="E33" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>895</v>
+      </c>
+      <c r="E34" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>899</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>897</v>
+      </c>
+      <c r="E36" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>901</v>
+      </c>
+      <c r="E37" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>901</v>
+      </c>
+      <c r="E38" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="C39">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>901</v>
+      </c>
+      <c r="E39" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="C40">
+        <v>7</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>895</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C41">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
+        <v>903</v>
+      </c>
+      <c r="E41" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="C42">
+        <v>7</v>
+      </c>
+      <c r="D42" t="s">
+        <v>907</v>
+      </c>
+      <c r="E42" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C43">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>877</v>
+      </c>
+      <c r="E43" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="C44">
+        <v>7</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>883</v>
+      </c>
+      <c r="E44" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="C45">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
+        <v>903</v>
+      </c>
+      <c r="E45" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="C46">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>877</v>
+      </c>
+      <c r="E46" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="C47">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>908</v>
+      </c>
+      <c r="E47" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="C48">
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>883</v>
+      </c>
+      <c r="E48" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="C49">
+        <v>7</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="C50">
+        <v>7</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="C51">
+        <v>7</v>
+      </c>
+      <c r="D51" t="s">
+        <v>909</v>
+      </c>
+      <c r="E51" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C52">
+        <v>7</v>
+      </c>
+      <c r="D52" t="s">
+        <v>910</v>
+      </c>
+      <c r="E52" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="C53">
+        <v>7</v>
+      </c>
+      <c r="D53" t="s">
+        <v>907</v>
+      </c>
+      <c r="E53" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="C54">
+        <v>7</v>
+      </c>
+      <c r="D54" t="s">
+        <v>877</v>
+      </c>
+      <c r="E54" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="C55">
+        <v>7</v>
+      </c>
+      <c r="D55" t="s">
+        <v>911</v>
+      </c>
+      <c r="E55" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="C56">
+        <v>7</v>
+      </c>
+      <c r="D56" t="s">
+        <v>912</v>
+      </c>
+      <c r="E56" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="C57">
+        <v>7</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>408</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="C58">
+        <v>7</v>
+      </c>
+      <c r="D58" t="s">
+        <v>908</v>
+      </c>
+      <c r="E58" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="C59">
+        <v>7</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>883</v>
+      </c>
+      <c r="E59" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="C60">
+        <v>8</v>
+      </c>
+      <c r="D60" t="s">
+        <v>876</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C61">
+        <v>8</v>
+      </c>
+      <c r="D61" t="s">
+        <v>882</v>
+      </c>
+      <c r="E61" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="C62">
+        <v>8</v>
+      </c>
+      <c r="D62" t="s">
+        <v>881</v>
+      </c>
+      <c r="E62" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C63">
+        <v>8</v>
+      </c>
+      <c r="D63" t="s">
+        <v>881</v>
+      </c>
+      <c r="E63" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="C64">
+        <v>8</v>
+      </c>
+      <c r="D64" t="s">
+        <v>876</v>
+      </c>
+      <c r="E64" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="C65">
+        <v>8</v>
+      </c>
+      <c r="D65" t="s">
+        <v>881</v>
+      </c>
+      <c r="E65" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="C66">
+        <v>8</v>
+      </c>
+      <c r="D66" t="s">
+        <v>876</v>
+      </c>
+      <c r="E66" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="C67">
+        <v>8</v>
+      </c>
+      <c r="D67" t="s">
+        <v>876</v>
+      </c>
+      <c r="E67" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="C68">
+        <v>8</v>
+      </c>
+      <c r="D68" t="s">
+        <v>881</v>
+      </c>
+      <c r="E68" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="C69">
+        <v>8</v>
+      </c>
+      <c r="D69" t="s">
+        <v>876</v>
+      </c>
+      <c r="E69" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="C70">
+        <v>8</v>
+      </c>
+      <c r="D70" t="s">
+        <v>882</v>
+      </c>
+      <c r="E70" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="C71">
+        <v>9</v>
+      </c>
+      <c r="D71" t="s">
+        <v>907</v>
+      </c>
+      <c r="E71" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="C72">
+        <v>9</v>
+      </c>
+      <c r="D72" t="s">
+        <v>907</v>
+      </c>
+      <c r="E72" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="C73">
+        <v>9</v>
+      </c>
+      <c r="D73" t="s">
+        <v>916</v>
+      </c>
+      <c r="E73" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="C74">
+        <v>9</v>
+      </c>
+      <c r="D74" t="s">
+        <v>916</v>
+      </c>
+      <c r="E74" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="C75">
+        <v>9</v>
+      </c>
+      <c r="D75" t="s">
+        <v>916</v>
+      </c>
+      <c r="E75" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="C76">
+        <v>10</v>
+      </c>
+      <c r="D76" t="s">
+        <v>918</v>
+      </c>
+      <c r="E76" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="C77">
+        <v>10</v>
+      </c>
+      <c r="D77" t="s">
+        <v>918</v>
+      </c>
+      <c r="E77" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C78">
+        <v>10</v>
+      </c>
+      <c r="D78" t="s">
+        <v>920</v>
+      </c>
+      <c r="E78" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="C79">
+        <v>10</v>
+      </c>
+      <c r="D79" t="s">
+        <v>918</v>
+      </c>
+      <c r="E79" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="C80">
+        <v>10</v>
+      </c>
+      <c r="D80" t="s">
+        <v>918</v>
+      </c>
+      <c r="E80" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="C81">
+        <v>10</v>
+      </c>
+      <c r="D81" t="s">
+        <v>920</v>
+      </c>
+      <c r="E81" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="C82">
+        <v>10</v>
+      </c>
+      <c r="D82" t="s">
+        <v>922</v>
+      </c>
+      <c r="E82" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="C83">
+        <v>10</v>
+      </c>
+      <c r="D83" t="s">
+        <v>922</v>
+      </c>
+      <c r="E83" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="C84">
+        <v>10</v>
+      </c>
+      <c r="D84" t="s">
+        <v>922</v>
+      </c>
+      <c r="E84" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="C85">
+        <v>10</v>
+      </c>
+      <c r="D85" t="s">
+        <v>918</v>
+      </c>
+      <c r="E85" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="C86">
+        <v>10</v>
+      </c>
+      <c r="D86" t="s">
+        <v>907</v>
+      </c>
+      <c r="E86" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C87">
+        <v>10</v>
+      </c>
+      <c r="D87" t="s">
+        <v>918</v>
+      </c>
+      <c r="E87" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C88">
+        <v>11</v>
+      </c>
+      <c r="D88" t="s">
+        <v>875</v>
+      </c>
+      <c r="E88" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="C89">
+        <v>11</v>
+      </c>
+      <c r="D89" t="s">
+        <v>875</v>
+      </c>
+      <c r="E89" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="C90">
+        <v>11</v>
+      </c>
+      <c r="D90" t="s">
+        <v>875</v>
+      </c>
+      <c r="E90" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="C91">
+        <v>11</v>
+      </c>
+      <c r="D91" t="s">
+        <v>924</v>
+      </c>
+      <c r="E91" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="C92">
+        <v>11</v>
+      </c>
+      <c r="D92" t="s">
+        <v>875</v>
+      </c>
+      <c r="E92" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="C93">
+        <v>12</v>
+      </c>
+      <c r="D93" t="s">
+        <v>926</v>
+      </c>
+      <c r="E93" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="C94">
+        <v>12</v>
+      </c>
+      <c r="D94" t="s">
+        <v>879</v>
+      </c>
+      <c r="E94" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="C95">
+        <v>12</v>
+      </c>
+      <c r="D95" t="s">
+        <v>922</v>
+      </c>
+      <c r="E95" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="C96">
+        <v>12</v>
+      </c>
+      <c r="D96" t="s">
+        <v>879</v>
+      </c>
+      <c r="E96" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C97">
+        <v>12</v>
+      </c>
+      <c r="D97" t="s">
+        <v>928</v>
+      </c>
+      <c r="E97" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="C98">
+        <v>12</v>
+      </c>
+      <c r="D98" t="s">
+        <v>930</v>
+      </c>
+      <c r="E98" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="C99">
+        <v>12</v>
+      </c>
+      <c r="D99" t="s">
+        <v>879</v>
+      </c>
+      <c r="E99" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="C100">
+        <v>12</v>
+      </c>
+      <c r="D100" s="13" t="s">
+        <v>932</v>
+      </c>
+      <c r="E100" s="13" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="C101">
+        <v>12</v>
+      </c>
+      <c r="D101" t="s">
+        <v>879</v>
+      </c>
+      <c r="E101" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="C102">
+        <v>12</v>
+      </c>
+      <c r="D102" t="s">
+        <v>933</v>
+      </c>
+      <c r="E102" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C103">
+        <v>12</v>
+      </c>
+      <c r="D103" t="s">
+        <v>930</v>
+      </c>
+      <c r="E103" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="C104">
+        <v>12</v>
+      </c>
+      <c r="D104" t="s">
+        <v>935</v>
+      </c>
+      <c r="E104" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="C105">
+        <v>13</v>
+      </c>
+      <c r="D105" t="s">
+        <v>928</v>
+      </c>
+      <c r="E105" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="C106">
+        <v>13</v>
+      </c>
+      <c r="D106" t="s">
+        <v>880</v>
+      </c>
+      <c r="E106" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="C107">
+        <v>13</v>
+      </c>
+      <c r="D107" t="s">
+        <v>936</v>
+      </c>
+      <c r="E107" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="C108">
+        <v>13</v>
+      </c>
+      <c r="D108" t="s">
+        <v>928</v>
+      </c>
+      <c r="E108" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="C109">
+        <v>14</v>
+      </c>
+      <c r="D109" t="s">
+        <v>878</v>
+      </c>
+      <c r="E109" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="C110">
+        <v>14</v>
+      </c>
+      <c r="D110" t="s">
+        <v>878</v>
+      </c>
+      <c r="E110" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="C111">
+        <v>14</v>
+      </c>
+      <c r="D111" t="s">
+        <v>878</v>
+      </c>
+      <c r="E111" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="C112">
+        <v>14</v>
+      </c>
+      <c r="D112" t="s">
+        <v>878</v>
+      </c>
+      <c r="E112" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="C113">
+        <v>15</v>
+      </c>
+      <c r="D113" t="s">
+        <v>938</v>
+      </c>
+      <c r="E113" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C114">
+        <v>15</v>
+      </c>
+      <c r="D114" t="s">
+        <v>938</v>
+      </c>
+      <c r="E114" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C115">
+        <v>15</v>
+      </c>
+      <c r="D115" t="s">
+        <v>938</v>
+      </c>
+      <c r="E115" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="C116">
+        <v>15</v>
+      </c>
+      <c r="D116" t="s">
+        <v>938</v>
+      </c>
+      <c r="E116" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="C117">
+        <v>15</v>
+      </c>
+      <c r="D117" t="s">
+        <v>938</v>
+      </c>
+      <c r="E117" t="s">
+        <v>937</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F118">
+    <sortCondition ref="C1:C118"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
# Korrektur der Wetterstation
</commit_message>
<xml_diff>
--- a/d/geo--comuni.xlsx
+++ b/d/geo--comuni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\PROGETTO\COVID\Covid-2\motioncharts\d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB851DAA-D0FB-4AE2-A194-6D731EA8B139}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465EC461-6846-4470-83E9-89153A749A1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="682" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3858" uniqueCount="940">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3857" uniqueCount="939">
   <si>
     <t>Chiave</t>
   </si>
@@ -2757,9 +2757,6 @@
   </si>
   <si>
     <t>Kaltern Oberplanitzing</t>
-  </si>
-  <si>
-    <t>Bozen(?)</t>
   </si>
   <si>
     <t>Barbian Kollmann</t>
@@ -18343,8 +18340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBDBBA6-5C55-4D9B-AB4F-2CB9A3B7975E}">
   <dimension ref="A1:F117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18370,7 +18367,7 @@
         <v>869</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -18842,10 +18839,10 @@
       <c r="C29">
         <v>4</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="14" t="s">
         <v>895</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="E29" s="14" t="s">
         <v>408</v>
       </c>
     </row>
@@ -18944,10 +18941,10 @@
       <c r="C35">
         <v>5</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="14" t="s">
         <v>899</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="E35" s="14" t="s">
         <v>900</v>
       </c>
     </row>
@@ -19029,10 +19026,10 @@
       <c r="C40">
         <v>7</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="14" t="s">
         <v>895</v>
       </c>
-      <c r="E40" s="13" t="s">
+      <c r="E40" s="14" t="s">
         <v>408</v>
       </c>
     </row>
@@ -19064,10 +19061,10 @@
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E42" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -19149,7 +19146,7 @@
         <v>7</v>
       </c>
       <c r="D47" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="E47" t="s">
         <v>578</v>
@@ -19217,7 +19214,7 @@
         <v>7</v>
       </c>
       <c r="D51" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E51" t="s">
         <v>586</v>
@@ -19234,7 +19231,7 @@
         <v>7</v>
       </c>
       <c r="D52" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="E52" t="s">
         <v>396</v>
@@ -19251,10 +19248,10 @@
         <v>7</v>
       </c>
       <c r="D53" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E53" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -19285,7 +19282,7 @@
         <v>7</v>
       </c>
       <c r="D55" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="E55" t="s">
         <v>420</v>
@@ -19302,10 +19299,10 @@
         <v>7</v>
       </c>
       <c r="D56" t="s">
+        <v>911</v>
+      </c>
+      <c r="E56" t="s">
         <v>912</v>
-      </c>
-      <c r="E56" t="s">
-        <v>913</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -19318,15 +19315,13 @@
       <c r="C57">
         <v>7</v>
       </c>
-      <c r="D57" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="E57" s="14" t="s">
-        <v>408</v>
-      </c>
-      <c r="F57" s="11" t="s">
-        <v>905</v>
-      </c>
+      <c r="D57" t="s">
+        <v>877</v>
+      </c>
+      <c r="E57" t="s">
+        <v>384</v>
+      </c>
+      <c r="F57" s="11"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
@@ -19339,7 +19334,7 @@
         <v>7</v>
       </c>
       <c r="D58" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="E58" t="s">
         <v>578</v>
@@ -19393,7 +19388,7 @@
         <v>882</v>
       </c>
       <c r="E61" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -19546,7 +19541,7 @@
         <v>882</v>
       </c>
       <c r="E70" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -19560,10 +19555,10 @@
         <v>9</v>
       </c>
       <c r="D71" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E71" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -19577,10 +19572,10 @@
         <v>9</v>
       </c>
       <c r="D72" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E72" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -19594,10 +19589,10 @@
         <v>9</v>
       </c>
       <c r="D73" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="E73" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -19611,10 +19606,10 @@
         <v>9</v>
       </c>
       <c r="D74" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="E74" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -19628,10 +19623,10 @@
         <v>9</v>
       </c>
       <c r="D75" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="E75" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -19645,10 +19640,10 @@
         <v>10</v>
       </c>
       <c r="D76" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="E76" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -19662,10 +19657,10 @@
         <v>10</v>
       </c>
       <c r="D77" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="E77" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -19679,10 +19674,10 @@
         <v>10</v>
       </c>
       <c r="D78" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="E78" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -19696,10 +19691,10 @@
         <v>10</v>
       </c>
       <c r="D79" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="E79" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -19713,10 +19708,10 @@
         <v>10</v>
       </c>
       <c r="D80" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="E80" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -19730,10 +19725,10 @@
         <v>10</v>
       </c>
       <c r="D81" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="E81" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -19747,10 +19742,10 @@
         <v>10</v>
       </c>
       <c r="D82" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="E82" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -19764,10 +19759,10 @@
         <v>10</v>
       </c>
       <c r="D83" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="E83" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -19781,10 +19776,10 @@
         <v>10</v>
       </c>
       <c r="D84" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="E84" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -19798,10 +19793,10 @@
         <v>10</v>
       </c>
       <c r="D85" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="E85" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -19815,10 +19810,10 @@
         <v>10</v>
       </c>
       <c r="D86" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E86" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -19832,10 +19827,10 @@
         <v>10</v>
       </c>
       <c r="D87" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="E87" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -19900,10 +19895,10 @@
         <v>11</v>
       </c>
       <c r="D91" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="E91" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -19934,10 +19929,10 @@
         <v>12</v>
       </c>
       <c r="D93" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="E93" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -19968,10 +19963,10 @@
         <v>12</v>
       </c>
       <c r="D95" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="E95" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -20002,10 +19997,10 @@
         <v>12</v>
       </c>
       <c r="D97" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="E97" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -20019,10 +20014,10 @@
         <v>12</v>
       </c>
       <c r="D98" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E98" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -20053,10 +20048,10 @@
         <v>12</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -20087,7 +20082,7 @@
         <v>12</v>
       </c>
       <c r="D102" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="E102" t="s">
         <v>548</v>
@@ -20104,10 +20099,10 @@
         <v>12</v>
       </c>
       <c r="D103" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E103" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -20121,10 +20116,10 @@
         <v>12</v>
       </c>
       <c r="D104" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="E104" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -20138,10 +20133,10 @@
         <v>13</v>
       </c>
       <c r="D105" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="E105" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -20172,7 +20167,7 @@
         <v>13</v>
       </c>
       <c r="D107" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="E107" t="s">
         <v>470</v>
@@ -20189,10 +20184,10 @@
         <v>13</v>
       </c>
       <c r="D108" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="E108" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -20274,10 +20269,10 @@
         <v>15</v>
       </c>
       <c r="D113" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="E113" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -20291,10 +20286,10 @@
         <v>15</v>
       </c>
       <c r="D114" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="E114" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -20308,10 +20303,10 @@
         <v>15</v>
       </c>
       <c r="D115" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="E115" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -20325,10 +20320,10 @@
         <v>15</v>
       </c>
       <c r="D116" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="E116" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -20342,10 +20337,10 @@
         <v>15</v>
       </c>
       <c r="D117" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="E117" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
   </sheetData>

</xml_diff>